<commit_message>
Implemented handling of ui with unique ids for definitions and locations
</commit_message>
<xml_diff>
--- a/TestEnvironment/TestCases.xlsx
+++ b/TestEnvironment/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\github\achimismaili\featureadmin\TestEnvironment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{401BB9BD-913D-438B-8249-A2B572731F57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{18A1DC60-3DC4-4C27-8ABA-61A5EB7AF10D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9555" activeTab="1" xr2:uid="{E8F90089-1E3D-48A9-A760-B45C82E8A33C}"/>
   </bookViews>
@@ -25,8 +25,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ismaili, Achim</author>
+  </authors>
+  <commentList>
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{009B3BC0-66F2-4787-9DA2-8375ABB1B6F7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ismaili, Achim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+(as this is only a demo, it is not implemented, that these activated features become faulty in case of a reload)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
   <si>
     <t>Areas</t>
   </si>
@@ -238,14 +272,121 @@
     <t>Saved Settings on</t>
   </si>
   <si>
-    <t>- activate a feature
+    <t>In detail view, properties should show "Elevated Privileges/Force true"</t>
+  </si>
+  <si>
+    <t>In detail view, properties should show "Elevated Privileges/Force false"</t>
+  </si>
+  <si>
+    <t>- Set 'Elevated Privileges' disabled and 'Force' disabled
+- activate a site or web feature
 - go to activated feature and show details</t>
   </si>
   <si>
-    <t>In detail view, properties should show "Elevated Privileges/Force true"</t>
-  </si>
-  <si>
-    <t>In detail view, properties should show "Elevated Privileges/Force false"</t>
+    <t>- Set 'Elevated Privileges' enabled and 'Force' enabled
+- activate a  site or web  feature
+- go to activated feature and show details</t>
+  </si>
+  <si>
+    <t>Filter Scope</t>
+  </si>
+  <si>
+    <t>Filter Feature name</t>
+  </si>
+  <si>
+    <t>Clear all filters in Feature Definition
+- Enter "content" in the search box</t>
+  </si>
+  <si>
+    <t>It should find plenty of feature defs and even one web app feature "Content Type Syndication"</t>
+  </si>
+  <si>
+    <t>- additionally to last test, select Option "web application" in Scope filter</t>
+  </si>
+  <si>
+    <t>Only one web app feature "Content Type Syndication" should be shown in results</t>
+  </si>
+  <si>
+    <t>Copy the Guid of Content Type Syndication via copy button on lower detail field
+- remove all filters
+- paste guid in search box</t>
+  </si>
+  <si>
+    <t>Filter Guid / copy button</t>
+  </si>
+  <si>
+    <t>Filter right</t>
+  </si>
+  <si>
+    <t>Only one web app feature def "Content Type Syndication" should be shown in results</t>
+  </si>
+  <si>
+    <t>Select web app feature def "Content Type Syndication" in result list</t>
+  </si>
+  <si>
+    <t>- Details are shown below
+- some properties can be copied to clipb.
+- Click on mag.glass shows window with details</t>
+  </si>
+  <si>
+    <t>34339dc9-dec4-4256-b44a-b30ff2991a64</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>Feature Def selection</t>
+  </si>
+  <si>
+    <t>Select web app feature def "Content Type Syndication" in result list
+- Click on "Filter right"</t>
+  </si>
+  <si>
+    <t>4 web apps should show up in locations result list, where this feature is activated</t>
+  </si>
+  <si>
+    <t>Select web app feature def "Content Type Syndication" in result list
+- Click on "Uninstall"</t>
+  </si>
+  <si>
+    <t>- confirmation dialog pops up to ask, if uninstall and also remove 4 active features
+- after confirm with yes, the feature definition and the 4 activated features do no longer show up in the results views</t>
+  </si>
+  <si>
+    <t>Log entries</t>
+  </si>
+  <si>
+    <t>- Restart feature admin
+- wait until farm load completed</t>
+  </si>
+  <si>
+    <t>- you should see different log entries with a warning having slightly thicker font
+- If log entries are bigger than window size, you should see a scrollbar to scroll up and down</t>
+  </si>
+  <si>
+    <t>Copy Log</t>
+  </si>
+  <si>
+    <t>Clear Log</t>
+  </si>
+  <si>
+    <t>- Restart feature admin
+- wait until farm load completed
+- Click 'Clear the Log' button</t>
+  </si>
+  <si>
+    <t>- Restart feature admin
+- wait until farm load completed
+- Click 'Copy Log' button
+- open text editor (e.g. notepad)
+- paste into editor</t>
+  </si>
+  <si>
+    <t>The content of the log should show up as text in the editor
+- The time format also contains the date</t>
+  </si>
+  <si>
+    <t>The log area is cleared and just the first prompt is shown, that log is active</t>
   </si>
 </sst>
 </file>
@@ -255,7 +396,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +419,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -328,10 +482,10 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -380,15 +534,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E984B914-F0FF-495B-8E39-00DFD973E50F}" name="Table1" displayName="Table1" ref="A4:F30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E984B914-F0FF-495B-8E39-00DFD973E50F}" name="Table1" displayName="Table1" ref="A4:F30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="1">
   <autoFilter ref="A4:F30" xr:uid="{97470821-C252-481A-B8D0-DBFAC18B3A87}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{50DD730F-7261-4428-A61D-70121C81DF3E}" name="Section" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{B1C1B2DB-F196-4027-BFFD-3F95FE7A6479}" name="System Under Test" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{5CE05041-5C29-4455-8B79-587D4F07C3F7}" name="Execute steps" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{1558C96C-AB89-4516-BAE9-170B5D105F60}" name="Test data" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{DCCAB690-0734-4A2D-9F19-6B9EE0099216}" name="Expected" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{287AD5BD-520C-4236-8C18-9BCEB3E8910A}" name="Result" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{DCCAB690-0734-4A2D-9F19-6B9EE0099216}" name="Expected" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{287AD5BD-520C-4236-8C18-9BCEB3E8910A}" name="Result" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{1558C96C-AB89-4516-BAE9-170B5D105F60}" name="Test data" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -911,20 +1065,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938FE77F-DD9B-40B6-8141-895BD8D6B4AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938FE77F-DD9B-40B6-8141-895BD8D6B4AD}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -967,16 +1121,16 @@
         <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -986,13 +1140,13 @@
       <c r="C5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>54</v>
       </c>
+      <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1002,13 +1156,13 @@
       <c r="C6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>54</v>
       </c>
+      <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -1018,13 +1172,13 @@
       <c r="C7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>58</v>
       </c>
+      <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1034,13 +1188,13 @@
       <c r="C8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>60</v>
       </c>
+      <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
@@ -1048,15 +1202,15 @@
         <v>62</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
@@ -1066,13 +1220,13 @@
       <c r="C10" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>61</v>
       </c>
+      <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
@@ -1080,71 +1234,111 @@
         <v>63</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
         <v>69</v>
       </c>
+      <c r="D11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
@@ -1188,31 +1382,51 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="B22" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
@@ -1249,7 +1463,9 @@
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1266,8 +1482,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed ActivatedFeatures not setting definition version
</commit_message>
<xml_diff>
--- a/TestEnvironment/TestCases.xlsx
+++ b/TestEnvironment/TestCases.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\github\achimismaili\featureadmin\TestEnvironment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{18A1DC60-3DC4-4C27-8ABA-61A5EB7AF10D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E09FC7BF-F67C-4F9D-BB10-0800ACF81D21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9555" activeTab="1" xr2:uid="{E8F90089-1E3D-48A9-A760-B45C82E8A33C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9555" activeTab="2" xr2:uid="{E8F90089-1E3D-48A9-A760-B45C82E8A33C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="UI" sheetId="2" r:id="rId2"/>
+    <sheet name="DataService" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
   <si>
     <t>Areas</t>
   </si>
@@ -394,7 +395,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -461,10 +462,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -480,12 +481,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -498,6 +496,48 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -534,17 +574,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E984B914-F0FF-495B-8E39-00DFD973E50F}" name="Table1" displayName="Table1" ref="A4:F30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E984B914-F0FF-495B-8E39-00DFD973E50F}" name="Table1" displayName="Table1" ref="A4:F30" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A4:F30" xr:uid="{97470821-C252-481A-B8D0-DBFAC18B3A87}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{50DD730F-7261-4428-A61D-70121C81DF3E}" name="Section" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B1C1B2DB-F196-4027-BFFD-3F95FE7A6479}" name="System Under Test" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{5CE05041-5C29-4455-8B79-587D4F07C3F7}" name="Execute steps" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{DCCAB690-0734-4A2D-9F19-6B9EE0099216}" name="Expected" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{287AD5BD-520C-4236-8C18-9BCEB3E8910A}" name="Result" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{1558C96C-AB89-4516-BAE9-170B5D105F60}" name="Test data" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{50DD730F-7261-4428-A61D-70121C81DF3E}" name="Section" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{B1C1B2DB-F196-4027-BFFD-3F95FE7A6479}" name="System Under Test" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{5CE05041-5C29-4455-8B79-587D4F07C3F7}" name="Execute steps" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{DCCAB690-0734-4A2D-9F19-6B9EE0099216}" name="Expected" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{287AD5BD-520C-4236-8C18-9BCEB3E8910A}" name="Result" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{1558C96C-AB89-4516-BAE9-170B5D105F60}" name="Test data" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15225B25-336B-4F08-BBB8-EE3839C84CA6}" name="Table13" displayName="Table13" ref="A4:F30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A4:F30" xr:uid="{97470821-C252-481A-B8D0-DBFAC18B3A87}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{0D6D0147-DCB9-4A51-B5C0-877AEDD48ABB}" name="Section" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{2B96925B-0A96-42AE-9EBB-6D14D18DE119}" name="System Under Test" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{CC21A0DF-C223-40DF-A75B-A19A86B8DE6B}" name="Execute steps" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{76C56721-2420-4AF5-92DD-065A41B11DF4}" name="Expected" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{5CAB1D28-7F4B-425E-821E-A25A8D55A65F}" name="Result" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{AD9A94C9-AC1B-4DC4-BCB3-316403D58A85}" name="Test data" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -847,7 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F4F674-A909-48CE-A10A-3F1131497C0D}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1068,7 +1123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938FE77F-DD9B-40B6-8141-895BD8D6B4AD}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -1487,4 +1542,286 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120BB734-656D-4E5D-9C35-D60A4370586A}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="5">
+        <v>43319</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Compatibility Level to feature definition result list
</commit_message>
<xml_diff>
--- a/TestEnvironment/TestCases.xlsx
+++ b/TestEnvironment/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\github\achimismaili\featureadmin\TestEnvironment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E09FC7BF-F67C-4F9D-BB10-0800ACF81D21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FEACF579-6DB2-4BAA-9403-2DE193A2BB88}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9555" activeTab="2" xr2:uid="{E8F90089-1E3D-48A9-A760-B45C82E8A33C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9555" activeTab="1" xr2:uid="{E8F90089-1E3D-48A9-A760-B45C82E8A33C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
   <si>
     <t>Areas</t>
   </si>
@@ -388,6 +388,87 @@
   </si>
   <si>
     <t>The log area is cleared and just the first prompt is shown, that log is active</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>Remove Activated Feature</t>
+  </si>
+  <si>
+    <t>Upgrade Activated Feature</t>
+  </si>
+  <si>
+    <t>Uninstall Definition</t>
+  </si>
+  <si>
+    <t>Read updated locations</t>
+  </si>
+  <si>
+    <t>Read updated definitions</t>
+  </si>
+  <si>
+    <t>Read updated act.features</t>
+  </si>
+  <si>
+    <t>Remove activated feature</t>
+  </si>
+  <si>
+    <t>Add Act. Feature force / el.p.</t>
+  </si>
+  <si>
+    <t>Add Act. Feature no force/el.p.</t>
+  </si>
+  <si>
+    <t>Uninstall Definition + remove af</t>
+  </si>
+  <si>
+    <t>Load a farm with locked sico</t>
+  </si>
+  <si>
+    <t>Load a farm with readonly sico</t>
+  </si>
+  <si>
+    <t>Load a farm with add content prevented sico</t>
+  </si>
+  <si>
+    <t>Load FA on non SharePoint computer</t>
+  </si>
+  <si>
+    <t>Load FA as non Admin</t>
+  </si>
+  <si>
+    <t>Load FA on SP2013</t>
+  </si>
+  <si>
+    <t>Load FA on SP2016</t>
+  </si>
+  <si>
+    <t>Load FA on SP2007 (WSS/MOSS)</t>
+  </si>
+  <si>
+    <t>Load FA on SP2010 (Found./Std)</t>
+  </si>
+  <si>
+    <t>Load FA on SP2019</t>
+  </si>
+  <si>
+    <t>Enabled buttons</t>
+  </si>
+  <si>
+    <t>Search for Guid</t>
+  </si>
+  <si>
+    <t>Show children</t>
+  </si>
+  <si>
+    <t>Show same ID</t>
+  </si>
+  <si>
+    <t>Show sandboxed defs</t>
   </si>
 </sst>
 </file>
@@ -574,8 +655,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E984B914-F0FF-495B-8E39-00DFD973E50F}" name="Table1" displayName="Table1" ref="A4:F30" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A4:F30" xr:uid="{97470821-C252-481A-B8D0-DBFAC18B3A87}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E984B914-F0FF-495B-8E39-00DFD973E50F}" name="Table1" displayName="Table1" ref="A4:F46" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A4:F46" xr:uid="{97470821-C252-481A-B8D0-DBFAC18B3A87}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{50DD730F-7261-4428-A61D-70121C81DF3E}" name="Section" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{B1C1B2DB-F196-4027-BFFD-3F95FE7A6479}" name="System Under Test" dataDxfId="12"/>
@@ -1121,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938FE77F-DD9B-40B6-8141-895BD8D6B4AD}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,7 +1482,9 @@
       <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1409,9 +1492,11 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1419,9 +1504,11 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1429,59 +1516,43 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>92</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>97</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>98</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
@@ -1494,24 +1565,36 @@
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1519,7 +1602,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1528,12 +1611,182 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1548,14 +1801,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120BB734-656D-4E5D-9C35-D60A4370586A}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="41.5703125" customWidth="1"/>
     <col min="4" max="4" width="41.140625" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
@@ -1611,80 +1864,120 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="C7" s="8"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="C8" s="8"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>106</v>
+      </c>
       <c r="C9" s="8"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="C10" s="8"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1699,87 +1992,129 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="C23" s="8"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="C24" s="8"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1787,7 +2122,9 @@
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+      <c r="A27" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1795,7 +2132,9 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1803,7 +2142,9 @@
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>

</xml_diff>

<commit_message>
filled out test cases for testing version 3.0.2
</commit_message>
<xml_diff>
--- a/TestEnvironment/TestCases.xlsx
+++ b/TestEnvironment/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\github\achimismaili\featureadmin\TestEnvironment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FEACF579-6DB2-4BAA-9403-2DE193A2BB88}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6EFD57CA-6764-4A22-A843-E00E1BE8E152}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9555" activeTab="1" xr2:uid="{E8F90089-1E3D-48A9-A760-B45C82E8A33C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9555" activeTab="2" xr2:uid="{E8F90089-1E3D-48A9-A760-B45C82E8A33C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="141">
   <si>
     <t>Areas</t>
   </si>
@@ -396,9 +396,6 @@
     <t>CRUD</t>
   </si>
   <si>
-    <t>Remove Activated Feature</t>
-  </si>
-  <si>
     <t>Upgrade Activated Feature</t>
   </si>
   <si>
@@ -469,6 +466,55 @@
   </si>
   <si>
     <t>Show sandboxed defs</t>
+  </si>
+  <si>
+    <t>Dialog window shows up to inform about demo mode</t>
+  </si>
+  <si>
+    <t>not implemented</t>
+  </si>
+  <si>
+    <t>FAILED
+Exception Error object …</t>
+  </si>
+  <si>
+    <t>User should be informed, that he does not have sufficient rights with link to web site</t>
+  </si>
+  <si>
+    <t>not tested</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Start FA as admin on a SP 2013 WFE</t>
+  </si>
+  <si>
+    <t>Feature Admin loads everything and works</t>
+  </si>
+  <si>
+    <t>Start FA as admin on a SP 2007 WFE</t>
+  </si>
+  <si>
+    <t>Start FA as admin on a SP 2010 WFE</t>
+  </si>
+  <si>
+    <t>Start FA as admin on a SP 2016 WFE</t>
+  </si>
+  <si>
+    <t>Start FA as admin on a SP 2019 WFE</t>
+  </si>
+  <si>
+    <t>ok (loaded in less than 2s)</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>3.0.2</t>
+  </si>
+  <si>
+    <t>(experimental)</t>
   </si>
 </sst>
 </file>
@@ -536,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -556,6 +602,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1204,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938FE77F-DD9B-40B6-8141-895BD8D6B4AD}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,6 +1274,9 @@
       <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
       <c r="E1" s="3" t="s">
         <v>50</v>
       </c>
@@ -1239,6 +1291,9 @@
       <c r="B2" t="s">
         <v>43</v>
       </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
       <c r="E2" s="3" t="s">
         <v>39</v>
       </c>
@@ -1279,8 +1334,10 @@
       <c r="D5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1295,7 +1352,9 @@
       <c r="D6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1311,7 +1370,9 @@
       <c r="D7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1327,7 +1388,9 @@
       <c r="D8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1343,7 +1406,9 @@
       <c r="D9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1359,7 +1424,9 @@
       <c r="D10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1375,7 +1442,9 @@
       <c r="D11" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1391,7 +1460,9 @@
       <c r="D12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F12" s="7" t="s">
         <v>84</v>
       </c>
@@ -1409,7 +1480,9 @@
       <c r="D13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1425,7 +1498,9 @@
       <c r="D14" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F14" s="7" t="s">
         <v>83</v>
       </c>
@@ -1443,7 +1518,9 @@
       <c r="D15" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1459,7 +1536,9 @@
       <c r="D16" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1475,7 +1554,9 @@
       <c r="D17" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1483,11 +1564,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1495,11 +1578,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1507,11 +1592,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1519,11 +1606,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1569,11 +1658,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1581,11 +1672,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+      <c r="E27" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1593,11 +1686,13 @@
         <v>5</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="E28" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1653,11 +1748,13 @@
         <v>6</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+      <c r="E34" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1665,11 +1762,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+      <c r="E35" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1685,7 +1784,9 @@
       <c r="D36" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="7"/>
+      <c r="E36" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1701,7 +1802,9 @@
       <c r="D37" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E37" s="7"/>
+      <c r="E37" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1717,7 +1820,9 @@
       <c r="D38" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1773,11 +1878,13 @@
         <v>9</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
+      <c r="E45" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1801,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120BB734-656D-4E5D-9C35-D60A4370586A}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,6 +1929,9 @@
       <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
       <c r="E1" s="3" t="s">
         <v>50</v>
       </c>
@@ -1836,11 +1946,14 @@
       <c r="B2" t="s">
         <v>43</v>
       </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
       <c r="E2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F2" s="5">
-        <v>43319</v>
+        <v>43353</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1868,11 +1981,13 @@
         <v>100</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1880,11 +1995,13 @@
         <v>100</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1892,7 +2009,7 @@
         <v>100</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="7"/>
@@ -1904,7 +2021,7 @@
         <v>100</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="7"/>
@@ -1916,7 +2033,7 @@
         <v>100</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="7"/>
@@ -1928,11 +2045,13 @@
         <v>100</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1940,11 +2059,13 @@
         <v>100</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1952,11 +2073,13 @@
         <v>100</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1964,20 +2087,20 @@
         <v>100</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>101</v>
-      </c>
+      <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1996,11 +2119,17 @@
         <v>99</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2008,11 +2137,17 @@
         <v>99</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+        <v>118</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2020,11 +2155,17 @@
         <v>99</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2032,11 +2173,17 @@
         <v>99</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+        <v>116</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2044,11 +2191,17 @@
         <v>99</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2056,7 +2209,7 @@
         <v>99</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -2068,7 +2221,7 @@
         <v>99</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2080,23 +2233,27 @@
         <v>99</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2104,11 +2261,15 @@
         <v>99</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>